<commit_message>
first row now working kako Bog zapovijeda
</commit_message>
<xml_diff>
--- a/Other files/Book1.xlsx
+++ b/Other files/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zgrubisic\Desktop\GIT_repositorys\demonstrature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zgrubisic\Desktop\GIT_repositorys\demonstrature\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="12570" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="12570" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -89,10 +89,13 @@
     <t>GroupTable</t>
   </si>
   <si>
-    <t>CourseID</t>
-  </si>
-  <si>
     <t>Owner</t>
+  </si>
+  <si>
+    <t>pr-lv1 i to</t>
+  </si>
+  <si>
+    <t>IDGroup</t>
   </si>
 </sst>
 </file>
@@ -129,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +461,7 @@
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -470,8 +474,11 @@
       <c r="J1" t="s">
         <v>20</v>
       </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -494,7 +501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -517,7 +524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -536,11 +543,8 @@
       <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -554,16 +558,16 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -577,22 +581,29 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>